<commit_message>
Add riskmanagment.pdf and usecase_doc.pdf
</commit_message>
<xml_diff>
--- a/SE2_Week 2/Riskmanagement.xlsx
+++ b/SE2_Week 2/Riskmanagement.xlsx
@@ -620,6 +620,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="B1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -926,7 +929,7 @@
     <sortCondition descending="1" ref="F2:F19"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="61" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>